<commit_message>
configurazione br e moduli nuovi 18-5-2017
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/test/RETAIL/test completamento br.xlsx
+++ b/earlywarning-pom/Document/test/RETAIL/test completamento br.xlsx
@@ -1184,11 +1184,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BV35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>